<commit_message>
fix: fix some interatctions and remove unused commands
</commit_message>
<xml_diff>
--- a/locale/locale.xlsx
+++ b/locale/locale.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="1137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="1133">
   <si>
     <t>langkey</t>
   </si>
@@ -2770,8 +2770,8 @@
     <t>register.dataurregistryaccount</t>
   </si>
   <si>
-    <t xml:space="preserve">{{{emoji_dota}}} {{dotaID}}
-{{{emoji_steam}}} {{steamID}}</t>
+    <t xml:space="preserve">{{{emoji_dota}}} {{{user_account_dota}}}
+{{{emoji_steam}}} {{{user_account_steam}}}</t>
   </si>
   <si>
     <t>register.help</t>
@@ -2801,13 +2801,11 @@
     <t>register.helpregistrydesc</t>
   </si>
   <si>
-    <t xml:space="preserve">:regional_indicator_h: :regional_indicator_e: :regional_indicator_l: :regional_indicator_p: Use `/help` to see availables commands.
-:information_source: You can use almost all commands by DM to **{{{bot_name}}}**!
+    <t xml:space="preserve">:information_source: You can use almost all commands by DM to **{{{bot_name}}}**!
 See your position in the bot ranking in {{{link_web_leaderboard}}}</t>
   </si>
   <si>
-    <t xml:space="preserve">:regional_indicator_h: :regional_indicator_e: :regional_indicator_l: :regional_indicator_p: Usa `/help` para ver los comandos disponibles.
-:information_source: ¡Puedes usar la mayoría de comandos por mensaje directo a **{{{bot_name}}}**!
+    <t xml:space="preserve">:information_source: ¡Puedes usar la mayoría de comandos por mensaje directo a **{{{bot_name}}}**!
 Mira tu posición en el ranking del bot en {{{link_web_leaderboard}}}</t>
   </si>
   <si>
@@ -2823,22 +2821,18 @@
     <t>registerAccountDesc</t>
   </si>
   <si>
-    <t xml:space="preserve">**Guild/DM:** `&lt;guildName&gt;` **ID:** `&lt;guildID&gt;`
-&lt;dota&gt; &lt;dotaID&gt;
-&lt;steam&gt; &lt;steamID&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Guild/DM:** `&lt;guildName&gt;` **ID:** `&lt;guildID&gt;`
-&lt;dota&gt; &lt;dotaID&gt;</t>
+    <t xml:space="preserve">**Guild/DM:** `{{{guild_name}}}` **ID:** `{{{guild_id}}}`
+{{{emoji_dota}}} {{{dotaID}}}
+{{{emoji_steam}}} {{{steamID}}}</t>
   </si>
   <si>
     <t>registerAccountTitle</t>
   </si>
   <si>
-    <t xml:space="preserve">Account registered - &lt;id&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registro de cuenta - &lt;id&gt;</t>
+    <t xml:space="preserve">Account registered - {{{user_account_id}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registro de cuenta - {{{user_account_id}}}</t>
   </si>
   <si>
     <t>roll.text</t>
@@ -2992,7 +2986,7 @@
     <t xml:space="preserve">:x: Mazos no encontrados con: `&lt;search&gt;`</t>
   </si>
   <si>
-    <t>searchplayer.description</t>
+    <t>search_player.description</t>
   </si>
   <si>
     <t xml:space="preserve">Search by: `{{{query}}}`
@@ -3003,7 +2997,7 @@
 {{{results}}}</t>
   </si>
   <si>
-    <t>searchplayer.footer</t>
+    <t>search_player.footer</t>
   </si>
   <si>
     <t xml:space="preserve">{{{count}}} results</t>
@@ -3012,7 +3006,7 @@
     <t xml:space="preserve">{{{count}}} resultados</t>
   </si>
   <si>
-    <t>searchplayer.mincharsrequired</t>
+    <t>search_player.mincharsrequired</t>
   </si>
   <si>
     <t xml:space="preserve">Mín. characters to search is `2`</t>
@@ -3021,7 +3015,7 @@
     <t xml:space="preserve">El mínimo de carácteres a buscar es `2`</t>
   </si>
   <si>
-    <t>searchplayer.title</t>
+    <t>search_player.title</t>
   </si>
   <si>
     <t xml:space="preserve">Search Players</t>
@@ -3030,13 +3024,13 @@
     <t xml:space="preserve">Búsqueda de Jugadores/as</t>
   </si>
   <si>
-    <t>searchpro.description</t>
-  </si>
-  <si>
-    <t>searchpro.footer</t>
-  </si>
-  <si>
-    <t>searchpro.title</t>
+    <t>search_pro.description</t>
+  </si>
+  <si>
+    <t>search_pro.footer</t>
+  </si>
+  <si>
+    <t>search_pro.title</t>
   </si>
   <si>
     <t xml:space="preserve">Pros search</t>
@@ -3045,7 +3039,7 @@
     <t xml:space="preserve">Búsqueda de Pros</t>
   </si>
   <si>
-    <t>searchworldranking.errorfind</t>
+    <t>search_worldranking.errorfind</t>
   </si>
   <si>
     <t xml:space="preserve">:x: It could find in World Ranking: `{{query}}`</t>
@@ -3054,16 +3048,7 @@
     <t xml:space="preserve">:x: No se ha podido encontrar en la clasificación mundial: `{{query}}`</t>
   </si>
   <si>
-    <t>searchworldranking.needquery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:x: It's neccesary to add a search text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:x: Es necesario añadir el término de búsqueda</t>
-  </si>
-  <si>
-    <t>searchworldranking.resultssearchquery</t>
+    <t>search_worldranking.resultssearchquery</t>
   </si>
   <si>
     <t xml:space="preserve">Search: `{{query}}`
@@ -3074,7 +3059,7 @@
 {{{results}}}</t>
   </si>
   <si>
-    <t>searchworldranking.searchplayer</t>
+    <t>search_worldranking.searchplayer</t>
   </si>
   <si>
     <t xml:space="preserve">Search player in World Ranking</t>
@@ -3630,7 +3615,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
@@ -3638,8 +3623,13 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4184,7 +4174,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A362" zoomScale="100" workbookViewId="0">
       <selection activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -4339,13 +4329,13 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -8113,36 +8103,36 @@
         <v>895</v>
       </c>
     </row>
-    <row r="361">
+    <row r="361" ht="33">
       <c r="A361" s="2" t="s">
         <v>896</v>
       </c>
-      <c r="B361" s="4" t="s">
+      <c r="B361" s="5" t="s">
         <v>897</v>
       </c>
-      <c r="C361" s="4" t="s">
+      <c r="C361" s="5" t="s">
         <v>897</v>
       </c>
     </row>
-    <row r="362">
+    <row r="362" ht="379.5">
       <c r="A362" s="2" t="s">
         <v>898</v>
       </c>
-      <c r="B362" t="s">
+      <c r="B362" s="4" t="s">
         <v>899</v>
       </c>
       <c r="C362" t="s">
         <v>900</v>
       </c>
     </row>
-    <row r="363">
+    <row r="363" ht="82.5">
       <c r="A363" s="2" t="s">
         <v>901</v>
       </c>
-      <c r="B363" s="4" t="s">
+      <c r="B363" s="5" t="s">
         <v>902</v>
       </c>
-      <c r="C363" s="4" t="s">
+      <c r="C363" s="5" t="s">
         <v>903</v>
       </c>
     </row>
@@ -8157,931 +8147,920 @@
         <v>906</v>
       </c>
     </row>
-    <row r="365">
+    <row r="365" ht="66">
       <c r="A365" s="2" t="s">
         <v>907</v>
       </c>
-      <c r="B365" t="s">
+      <c r="B365" s="4" t="s">
         <v>908</v>
       </c>
-      <c r="C365" t="s">
-        <v>909</v>
+      <c r="C365" s="4" t="s">
+        <v>908</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="B366" t="s">
         <v>910</v>
       </c>
-      <c r="B366" t="s">
+      <c r="C366" t="s">
         <v>911</v>
-      </c>
-      <c r="C366" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="B367" t="s">
         <v>913</v>
       </c>
-      <c r="B367" t="s">
+      <c r="C367" t="s">
         <v>914</v>
-      </c>
-      <c r="C367" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="B368" t="s">
         <v>916</v>
       </c>
-      <c r="B368" t="s">
+      <c r="C368" t="s">
         <v>917</v>
-      </c>
-      <c r="C368" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="B369" t="s">
         <v>919</v>
       </c>
-      <c r="B369" t="s">
-        <v>920</v>
-      </c>
       <c r="C369" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B370" t="s">
         <v>921</v>
       </c>
-      <c r="B370" t="s">
-        <v>922</v>
-      </c>
       <c r="C370" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="B371" t="s">
         <v>923</v>
       </c>
-      <c r="B371" t="s">
+      <c r="C371" t="s">
         <v>924</v>
-      </c>
-      <c r="C371" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="B372" t="s">
         <v>926</v>
       </c>
-      <c r="B372" t="s">
+      <c r="C372" t="s">
         <v>927</v>
-      </c>
-      <c r="C372" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="B373" t="s">
         <v>929</v>
       </c>
-      <c r="B373" t="s">
-        <v>930</v>
-      </c>
       <c r="C373" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="B374" t="s">
         <v>931</v>
       </c>
-      <c r="B374" t="s">
+      <c r="C374" t="s">
         <v>932</v>
-      </c>
-      <c r="C374" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="B375" t="s">
         <v>934</v>
       </c>
-      <c r="B375" t="s">
+      <c r="C375" t="s">
         <v>935</v>
-      </c>
-      <c r="C375" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="B376" t="s">
         <v>937</v>
       </c>
-      <c r="B376" t="s">
+      <c r="C376" t="s">
         <v>938</v>
-      </c>
-      <c r="C376" t="s">
-        <v>939</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="B377" t="s">
         <v>940</v>
       </c>
-      <c r="B377" t="s">
+      <c r="C377" t="s">
         <v>941</v>
-      </c>
-      <c r="C377" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="B378" t="s">
         <v>943</v>
       </c>
-      <c r="B378" t="s">
+      <c r="C378" t="s">
         <v>944</v>
-      </c>
-      <c r="C378" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="2" t="s">
+        <v>945</v>
+      </c>
+      <c r="B379" t="s">
         <v>946</v>
       </c>
-      <c r="B379" t="s">
+      <c r="C379" t="s">
         <v>947</v>
-      </c>
-      <c r="C379" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="B380" t="s">
         <v>949</v>
       </c>
-      <c r="B380" t="s">
+      <c r="C380" t="s">
         <v>950</v>
-      </c>
-      <c r="C380" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="2" t="s">
+        <v>951</v>
+      </c>
+      <c r="B381" t="s">
         <v>952</v>
       </c>
-      <c r="B381" t="s">
+      <c r="C381" t="s">
         <v>953</v>
-      </c>
-      <c r="C381" t="s">
-        <v>954</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="B382" t="s">
         <v>955</v>
       </c>
-      <c r="B382" t="s">
+      <c r="C382" t="s">
         <v>956</v>
       </c>
-      <c r="C382" t="s">
+    </row>
+    <row r="383" ht="49.5">
+      <c r="A383" s="6" t="s">
         <v>957</v>
       </c>
-    </row>
-    <row r="383">
-      <c r="A383" s="2" t="s">
+      <c r="B383" s="4" t="s">
         <v>958</v>
       </c>
-      <c r="B383" s="4" t="s">
+      <c r="C383" s="4" t="s">
         <v>959</v>
       </c>
-      <c r="C383" s="4" t="s">
+    </row>
+    <row r="384">
+      <c r="A384" s="6" t="s">
         <v>960</v>
       </c>
-    </row>
-    <row r="384">
-      <c r="A384" s="2" t="s">
+      <c r="B384" t="s">
         <v>961</v>
       </c>
-      <c r="B384" t="s">
+      <c r="C384" t="s">
         <v>962</v>
       </c>
-      <c r="C384" t="s">
+    </row>
+    <row r="385">
+      <c r="A385" s="6" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="385">
-      <c r="A385" s="2" t="s">
+      <c r="B385" t="s">
         <v>964</v>
       </c>
-      <c r="B385" t="s">
+      <c r="C385" t="s">
         <v>965</v>
       </c>
-      <c r="C385" t="s">
+    </row>
+    <row r="386">
+      <c r="A386" s="6" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="386">
-      <c r="A386" s="2" t="s">
+      <c r="B386" t="s">
         <v>967</v>
       </c>
-      <c r="B386" t="s">
+      <c r="C386" t="s">
         <v>968</v>
       </c>
-      <c r="C386" t="s">
+    </row>
+    <row r="387" ht="49.5">
+      <c r="A387" s="6" t="s">
         <v>969</v>
       </c>
-    </row>
-    <row r="387" ht="49.5">
-      <c r="A387" s="2" t="s">
+      <c r="B387" s="4" t="s">
+        <v>958</v>
+      </c>
+      <c r="C387" s="4" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="6" t="s">
         <v>970</v>
       </c>
-      <c r="B387" s="4" t="s">
-        <v>959</v>
-      </c>
-      <c r="C387" s="4" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="388">
-      <c r="A388" s="2" t="s">
+      <c r="B388" t="s">
+        <v>961</v>
+      </c>
+      <c r="C388" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="6" t="s">
         <v>971</v>
       </c>
-      <c r="B388" t="s">
-        <v>962</v>
-      </c>
-      <c r="C388" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="389">
-      <c r="A389" s="2" t="s">
+      <c r="B389" t="s">
         <v>972</v>
       </c>
-      <c r="B389" t="s">
+      <c r="C389" t="s">
         <v>973</v>
-      </c>
-      <c r="C389" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="B390" s="7" t="s">
         <v>975</v>
       </c>
-      <c r="B390" t="s">
+      <c r="C390" s="7" t="s">
         <v>976</v>
-      </c>
-      <c r="C390" t="s">
-        <v>977</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="B391" s="4" t="s">
         <v>978</v>
       </c>
-      <c r="B391" t="s">
+      <c r="C391" s="4" t="s">
         <v>979</v>
       </c>
-      <c r="C391" t="s">
+    </row>
+    <row r="392">
+      <c r="A392" s="2" t="s">
         <v>980</v>
       </c>
-    </row>
-    <row r="392" ht="49.5">
-      <c r="A392" s="2" t="s">
+      <c r="B392" s="7" t="s">
         <v>981</v>
       </c>
-      <c r="B392" s="4" t="s">
+      <c r="C392" s="7" t="s">
         <v>982</v>
-      </c>
-      <c r="C392" s="4" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="B393" t="s">
         <v>984</v>
       </c>
-      <c r="B393" t="s">
-        <v>985</v>
-      </c>
       <c r="C393" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="2" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="B394" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="C394" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="B395" t="s">
+        <v>988</v>
+      </c>
+      <c r="C395" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="396" ht="33">
+      <c r="A396" s="2" t="s">
         <v>989</v>
       </c>
-      <c r="B395" t="s">
+      <c r="B396" s="4" t="s">
         <v>990</v>
       </c>
-      <c r="C395" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="396">
-      <c r="A396" s="2" t="s">
+      <c r="C396" t="s">
         <v>991</v>
       </c>
-      <c r="B396" t="s">
+    </row>
+    <row r="397">
+      <c r="A397" s="2" t="s">
         <v>992</v>
       </c>
-      <c r="C396" t="s">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="397" ht="33">
-      <c r="A397" s="2" t="s">
+      <c r="B397" t="s">
         <v>993</v>
       </c>
-      <c r="B397" s="4" t="s">
+      <c r="C397" t="s">
         <v>994</v>
-      </c>
-      <c r="C397" t="s">
-        <v>995</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="B398" t="s">
         <v>996</v>
       </c>
-      <c r="B398" t="s">
+      <c r="C398" t="s">
         <v>997</v>
-      </c>
-      <c r="C398" t="s">
-        <v>998</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="B399" t="s">
         <v>999</v>
       </c>
-      <c r="B399" t="s">
-        <v>1000</v>
-      </c>
       <c r="C399" t="s">
-        <v>1001</v>
+        <v>435</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="2" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B400" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C400" t="s">
         <v>1002</v>
-      </c>
-      <c r="B400" t="s">
-        <v>1003</v>
-      </c>
-      <c r="C400" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="2" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B401" t="s">
         <v>1004</v>
       </c>
-      <c r="B401" t="s">
+      <c r="C401" t="s">
         <v>1005</v>
-      </c>
-      <c r="C401" t="s">
-        <v>1006</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="2" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B402" t="s">
+        <v>472</v>
+      </c>
+      <c r="C402" t="s">
         <v>1007</v>
-      </c>
-      <c r="B402" t="s">
-        <v>1008</v>
-      </c>
-      <c r="C402" t="s">
-        <v>1009</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B403" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C403" t="s">
         <v>1010</v>
       </c>
-      <c r="B403" t="s">
-        <v>472</v>
-      </c>
-      <c r="C403" t="s">
+    </row>
+    <row r="404" ht="33">
+      <c r="A404" s="2" t="s">
         <v>1011</v>
       </c>
-    </row>
-    <row r="404">
-      <c r="A404" s="2" t="s">
+      <c r="B404" s="4" t="s">
         <v>1012</v>
       </c>
-      <c r="B404" t="s">
+      <c r="C404" s="4" t="s">
         <v>1013</v>
       </c>
-      <c r="C404" t="s">
+    </row>
+    <row r="405">
+      <c r="A405" s="2" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="405" ht="33">
-      <c r="A405" s="2" t="s">
+      <c r="B405" t="s">
         <v>1015</v>
       </c>
-      <c r="B405" s="4" t="s">
-        <v>1016</v>
-      </c>
-      <c r="C405" s="4" t="s">
-        <v>1017</v>
+      <c r="C405" t="s">
+        <v>1015</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="2" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="B406" t="s">
-        <v>1019</v>
+        <v>143</v>
       </c>
       <c r="C406" t="s">
-        <v>1019</v>
+        <v>143</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="2" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="B407" t="s">
-        <v>143</v>
+        <v>1018</v>
       </c>
       <c r="C407" t="s">
-        <v>143</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="2" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B408" t="s">
-        <v>1022</v>
+        <v>513</v>
       </c>
       <c r="C408" t="s">
-        <v>1023</v>
+        <v>514</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="2" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="B409" t="s">
-        <v>513</v>
+        <v>1022</v>
       </c>
       <c r="C409" t="s">
-        <v>514</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="2" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B410" t="s">
         <v>1025</v>
       </c>
-      <c r="B410" t="s">
+      <c r="C410" t="s">
         <v>1026</v>
-      </c>
-      <c r="C410" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B411" t="s">
         <v>1028</v>
       </c>
-      <c r="B411" t="s">
+      <c r="C411" t="s">
         <v>1029</v>
-      </c>
-      <c r="C411" t="s">
-        <v>1030</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B412" t="s">
         <v>1031</v>
       </c>
-      <c r="B412" t="s">
+      <c r="C412" t="s">
         <v>1032</v>
-      </c>
-      <c r="C412" t="s">
-        <v>1033</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="2" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B413" t="s">
         <v>1034</v>
       </c>
-      <c r="B413" t="s">
+      <c r="C413" t="s">
         <v>1035</v>
-      </c>
-      <c r="C413" t="s">
-        <v>1036</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="2" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B414" t="s">
         <v>1037</v>
       </c>
-      <c r="B414" t="s">
+      <c r="C414" t="s">
         <v>1038</v>
-      </c>
-      <c r="C414" t="s">
-        <v>1039</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B415" t="s">
         <v>1040</v>
       </c>
-      <c r="B415" t="s">
+      <c r="C415" t="s">
         <v>1041</v>
-      </c>
-      <c r="C415" t="s">
-        <v>1042</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B416" t="s">
         <v>1043</v>
       </c>
-      <c r="B416" t="s">
+      <c r="C416" t="s">
         <v>1044</v>
-      </c>
-      <c r="C416" t="s">
-        <v>1045</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="2" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B417" t="s">
         <v>1046</v>
       </c>
-      <c r="B417" t="s">
+      <c r="C417" t="s">
         <v>1047</v>
-      </c>
-      <c r="C417" t="s">
-        <v>1048</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B418" t="s">
         <v>1049</v>
       </c>
-      <c r="B418" t="s">
+      <c r="C418" t="s">
         <v>1050</v>
-      </c>
-      <c r="C418" t="s">
-        <v>1051</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B419" t="s">
+        <v>711</v>
+      </c>
+      <c r="C419" t="s">
         <v>1052</v>
-      </c>
-      <c r="B419" t="s">
-        <v>1053</v>
-      </c>
-      <c r="C419" t="s">
-        <v>1054</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="2" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="B420" t="s">
-        <v>711</v>
+        <v>609</v>
       </c>
       <c r="C420" t="s">
-        <v>1056</v>
+        <v>610</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="2" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="B421" t="s">
-        <v>609</v>
+        <v>1055</v>
       </c>
       <c r="C421" t="s">
-        <v>610</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="2" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B422" t="s">
         <v>1058</v>
       </c>
-      <c r="B422" t="s">
+      <c r="C422" t="s">
         <v>1059</v>
-      </c>
-      <c r="C422" t="s">
-        <v>1060</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="2" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B423" t="s">
         <v>1061</v>
       </c>
-      <c r="B423" t="s">
+      <c r="C423" t="s">
         <v>1062</v>
-      </c>
-      <c r="C423" t="s">
-        <v>1063</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B424" t="s">
         <v>1064</v>
       </c>
-      <c r="B424" t="s">
+      <c r="C424" t="s">
         <v>1065</v>
-      </c>
-      <c r="C424" t="s">
-        <v>1066</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="2" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B425" t="s">
         <v>1067</v>
       </c>
-      <c r="B425" t="s">
+      <c r="C425" t="s">
         <v>1068</v>
-      </c>
-      <c r="C425" t="s">
-        <v>1069</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B426" t="s">
         <v>1070</v>
       </c>
-      <c r="B426" t="s">
+      <c r="C426" t="s">
         <v>1071</v>
-      </c>
-      <c r="C426" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="2" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B427" t="s">
         <v>1073</v>
       </c>
-      <c r="B427" t="s">
+      <c r="C427" t="s">
         <v>1074</v>
-      </c>
-      <c r="C427" t="s">
-        <v>1075</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="2" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B428" t="s">
         <v>1076</v>
       </c>
-      <c r="B428" t="s">
+      <c r="C428" t="s">
         <v>1077</v>
-      </c>
-      <c r="C428" t="s">
-        <v>1078</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="2" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B429" t="s">
         <v>1079</v>
       </c>
-      <c r="B429" t="s">
+      <c r="C429" t="s">
         <v>1080</v>
-      </c>
-      <c r="C429" t="s">
-        <v>1081</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="2" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B430" t="s">
         <v>1082</v>
       </c>
-      <c r="B430" t="s">
+      <c r="C430" t="s">
         <v>1083</v>
-      </c>
-      <c r="C430" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B431" t="s">
         <v>1085</v>
       </c>
-      <c r="B431" t="s">
+      <c r="C431" t="s">
         <v>1086</v>
-      </c>
-      <c r="C431" t="s">
-        <v>1087</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="2" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B432" t="s">
         <v>1088</v>
       </c>
-      <c r="B432" t="s">
-        <v>1089</v>
-      </c>
       <c r="C432" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="2" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B433" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C433" t="s">
         <v>1091</v>
-      </c>
-      <c r="B433" t="s">
-        <v>1092</v>
-      </c>
-      <c r="C433" t="s">
-        <v>1092</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="2" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B434" t="s">
         <v>1093</v>
       </c>
-      <c r="B434" t="s">
+      <c r="C434" t="s">
         <v>1094</v>
-      </c>
-      <c r="C434" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="2" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B435" t="s">
         <v>1096</v>
       </c>
-      <c r="B435" t="s">
-        <v>1097</v>
-      </c>
       <c r="C435" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="2" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B436" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C436" t="s">
         <v>1099</v>
-      </c>
-      <c r="B436" t="s">
-        <v>1100</v>
-      </c>
-      <c r="C436" t="s">
-        <v>1100</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="2" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B437" t="s">
         <v>1101</v>
       </c>
-      <c r="B437" t="s">
+      <c r="C437" t="s">
         <v>1102</v>
-      </c>
-      <c r="C437" t="s">
-        <v>1103</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="2" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B438" t="s">
         <v>1104</v>
       </c>
-      <c r="B438" t="s">
+      <c r="C438" t="s">
         <v>1105</v>
-      </c>
-      <c r="C438" t="s">
-        <v>1106</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="2" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B439" t="s">
         <v>1107</v>
       </c>
-      <c r="B439" t="s">
+      <c r="C439" t="s">
         <v>1108</v>
-      </c>
-      <c r="C439" t="s">
-        <v>1109</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="2" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B440" t="s">
         <v>1110</v>
       </c>
-      <c r="B440" t="s">
+      <c r="C440" t="s">
         <v>1111</v>
-      </c>
-      <c r="C440" t="s">
-        <v>1112</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="2" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B441" s="3" t="s">
         <v>1113</v>
       </c>
-      <c r="B441" t="s">
+      <c r="C441" t="s">
         <v>1114</v>
-      </c>
-      <c r="C441" t="s">
-        <v>1115</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="2" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B442" t="s">
         <v>1116</v>
       </c>
-      <c r="B442" s="3" t="s">
+      <c r="C442" t="s">
         <v>1117</v>
       </c>
-      <c r="C442" t="s">
+    </row>
+    <row r="443" ht="33">
+      <c r="A443" s="2" t="s">
         <v>1118</v>
       </c>
-    </row>
-    <row r="443">
-      <c r="A443" s="2" t="s">
+      <c r="B443" s="4" t="s">
         <v>1119</v>
       </c>
-      <c r="B443" t="s">
+      <c r="C443" s="4" t="s">
         <v>1120</v>
       </c>
-      <c r="C443" t="s">
+    </row>
+    <row r="444">
+      <c r="A444" s="2" t="s">
         <v>1121</v>
       </c>
-    </row>
-    <row r="444" ht="33">
-      <c r="A444" s="2" t="s">
+      <c r="B444" t="s">
         <v>1122</v>
       </c>
-      <c r="B444" s="4" t="s">
+      <c r="C444" t="s">
         <v>1123</v>
-      </c>
-      <c r="C444" s="4" t="s">
-        <v>1124</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="2" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B445" t="s">
         <v>1125</v>
       </c>
-      <c r="B445" t="s">
+      <c r="C445" t="s">
         <v>1126</v>
       </c>
-      <c r="C445" t="s">
+    </row>
+    <row r="446" ht="409.5">
+      <c r="A446" s="2" t="s">
         <v>1127</v>
       </c>
-    </row>
-    <row r="446">
-      <c r="A446" s="2" t="s">
+      <c r="B446" s="4" t="s">
         <v>1128</v>
       </c>
-      <c r="B446" t="s">
+      <c r="C446" s="4" t="s">
         <v>1129</v>
-      </c>
-      <c r="C446" t="s">
-        <v>1130</v>
       </c>
     </row>
     <row r="447" ht="409.5">
       <c r="A447" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B447" s="4" t="s">
         <v>1131</v>
       </c>
-      <c r="B447" s="4" t="s">
+      <c r="C447" s="4" t="s">
         <v>1132</v>
       </c>
-      <c r="C447" s="4" t="s">
-        <v>1133</v>
-      </c>
-    </row>
-    <row r="448" ht="409.5">
-      <c r="A448" s="2" t="s">
-        <v>1134</v>
-      </c>
-      <c r="B448" s="4" t="s">
-        <v>1135</v>
-      </c>
-      <c r="C448" s="4" t="s">
-        <v>1136</v>
-      </c>
-    </row>
-    <row r="449" ht="16.5"/>
+    </row>
+    <row r="448" ht="16.5"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>